<commit_message>
Downloaded 800m PRISM data but it is virtually the same as 4km
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/02_monitoring-events-with-PRISM-csv-file-name.xlsx
+++ b/data/data-wrangling-intermediate/02_monitoring-events-with-PRISM-csv-file-name.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/03_Buffelgrass CHNS/Buffelgrass_precip-variation/data/data-wrangling-intermediate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltnmsu-my.sharepoint.com/personal/lossanna_nmsu_edu/Documents/Documents/01_Buffelgrass/Buffelgrass_precip-variation/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="8_{E6624D43-6562-40FF-8EBF-8675BFEB0D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6812A811-E24F-48CE-8E81-959AEB3298B7}"/>
+  <xr:revisionPtr revIDLastSave="287" documentId="8_{E6624D43-6562-40FF-8EBF-8675BFEB0D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E4FFF7-08C7-4C67-8505-BF5D7328D65B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{C691EA87-9DF1-4D7D-ACFC-EEBD4FB4EF27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{C691EA87-9DF1-4D7D-ACFC-EEBD4FB4EF27}"/>
   </bookViews>
   <sheets>
-    <sheet name="daily" sheetId="1" r:id="rId1"/>
-    <sheet name="normals" sheetId="2" r:id="rId2"/>
+    <sheet name="daily_800m" sheetId="3" r:id="rId1"/>
+    <sheet name="daily_4km" sheetId="1" r:id="rId2"/>
+    <sheet name="normals" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="244">
   <si>
     <t>Site</t>
   </si>
@@ -523,6 +524,252 @@
   </si>
   <si>
     <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_monthly_normals_32.2838_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200928_20210928_32.2486_-111.1804.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211101_20221101_32.2486_-111.1804.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200929_20210929_32.2486_-111.1797.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211101_20221101_32.2486_-111.1797.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200912_20210912_32.2490_-111.1792.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211111_20221111_32.2490_-111.1792.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200911_20210911_32.2496_-111.1812.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211104_20221104_32.2496_-111.1812.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200911_20210911_32.2490_-111.1817.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211104_20221104_32.2490_-111.1817.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200912_20210912_32.2490_-111.1789.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211111_20221111_32.2490_-111.1789.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200929_20210929_32.2501_-111.1835.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211111_20221111_32.2501_-111.1835.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201015_20211015_32.2834_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211011_20221011_32.2834_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221103_20231103_32.2834_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201002_20211002_32.2838_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211017_20221017_32.2838_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221027_20231027_32.2838_-111.1922.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201008_20211008_32.2843_-111.1906.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211113_20221113_32.2843_-111.1906.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211018_20221018_32.2843_-111.1906.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221108_20231108_32.2843_-111.1906.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201002_20211002_32.2839_-111.1925.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211011_20221011_32.2839_-111.1925.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221101_20231101_32.2839_-111.1925.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201002_20211002_32.2842_-111.1919.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211017_20221017_32.2842_-111.1919.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221106_20231106_32.2842_-111.1919.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201003_20211003_32.2843_-111.1931.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211018_20221018_32.2843_-111.1931.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221110_20231110_32.2843_-111.1931.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201023_20211023_32.1919_-110.6981.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211123_20221123_32.1919_-110.6981.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221211_20231211_32.1919_-110.6981.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201009_20211009_32.1917_-110.6965.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211122_20221122_32.1917_-110.6965.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221213_20231213_32.1917_-110.6965.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201009_20211009_32.1916_-110.6963.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211122_20221122_32.1916_-110.6963.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20221215_20231215_32.1916_-110.6963.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191001_20201001_32.2150_-111.0088.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191019_20201019_32.2150_-111.0088.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201025_20211025_32.2150_-111.0088.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211128_20221128_32.2150_-111.0088.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191019_20201019_32.2125_-111.0093.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201014_20211014_32.2125_-111.0093.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211129_20221129_32.2125_-111.0093.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191001_20201001_32.2156_-111.0081.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200925_20210925_32.2156_-111.0081.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211129_20221129_32.2156_-111.0081.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191016_20201016_32.2178_-111.0075.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200926_20210926_32.2178_-111.0075.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211115_20221115_32.2178_-111.0075.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20190928_20200928_32.2176_-111.0074.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200926_20210926_32.2176_-111.0074.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211115_20221115_32.2176_-111.0074.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20190930_20200930_32.2163_-111.0065.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20190928_20200928_32.2163_-111.0065.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200925_20210925_32.2163_-111.0065.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211114_20221114_32.2163_-111.0065.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191013_20201013_32.2103_-111.0059.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201010_20211010_32.2103_-111.0059.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211205_20221205_32.2103_-111.0059.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191015_20201015_32.2094_-111.0061.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201010_20211010_32.2094_-111.0061.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20211205_20221205_32.2094_-111.0061.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20190929_20200929_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191017_20201017_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200924_20210924_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201027_20211027_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201101_20211101_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201026_20211026_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201028_20211028_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201029_20211029_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201030_20211030_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201031_20211031_32.2138_-111.0029.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20190929_20200929_32.2149_-111.0021.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20200925_20210925_32.2149_-111.0021.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20191012_20201012_32.2111_-111.0045.csv</t>
+  </si>
+  <si>
+    <t>PRISM_ppt_tmin_tmean_tmax_stable_800m_20201026_20211026_32.2111_-111.0045.csv</t>
   </si>
 </sst>
 </file>
@@ -585,6 +832,104 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>32385</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>382905</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E73EA50-3096-40E3-B8F2-C386F113FC33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13729335" y="323850"/>
+          <a:ext cx="3398520" cy="2118360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> is the list of monitoring events (unique site-transect and date), along with the corresponding CSV with PRISM data. The time period ranges from one year before the sampling date, which will be Prev_year_precip.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Precip values of each CSV are summed in 02.1.R.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Daily values downloaded at 800 m resolution (became freely available as of March 2025).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -664,6 +1009,15 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>Precip values of each CSV are summed in 02.1.R.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Daily values downloaded at 4 km resolution.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -671,6 +1025,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -989,25 +1347,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70659E3-6ADF-4861-A423-05040D976FDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6ADD30-E31B-4235-9B9A-CA0898EFFDC4}">
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K83" sqref="K83"/>
+      <selection pane="bottomLeft" activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1074,10 +1432,10 @@
         <v>26</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1109,10 +1467,10 @@
         <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1144,10 +1502,10 @@
         <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1179,10 +1537,10 @@
         <v>29</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1214,10 +1572,10 @@
         <v>30</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1249,10 +1607,10 @@
         <v>30</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1284,10 +1642,10 @@
         <v>31</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1319,10 +1677,10 @@
         <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1354,10 +1712,10 @@
         <v>32</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1389,10 +1747,10 @@
         <v>32</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1424,10 +1782,10 @@
         <v>33</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1459,10 +1817,10 @@
         <v>33</v>
       </c>
       <c r="K13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1494,10 +1852,10 @@
         <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1529,10 +1887,10 @@
         <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1564,10 +1922,10 @@
         <v>35</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1599,10 +1957,10 @@
         <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1634,10 +1992,10 @@
         <v>35</v>
       </c>
       <c r="K18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1669,10 +2027,10 @@
         <v>36</v>
       </c>
       <c r="K19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1704,10 +2062,10 @@
         <v>36</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1739,10 +2097,10 @@
         <v>36</v>
       </c>
       <c r="K21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1774,10 +2132,10 @@
         <v>37</v>
       </c>
       <c r="K22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1809,10 +2167,10 @@
         <v>37</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1844,10 +2202,10 @@
         <v>37</v>
       </c>
       <c r="K24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1879,10 +2237,10 @@
         <v>37</v>
       </c>
       <c r="K25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1914,10 +2272,10 @@
         <v>38</v>
       </c>
       <c r="K26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1949,10 +2307,10 @@
         <v>38</v>
       </c>
       <c r="K27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1984,10 +2342,10 @@
         <v>38</v>
       </c>
       <c r="K28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2019,10 +2377,10 @@
         <v>39</v>
       </c>
       <c r="K29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -2054,10 +2412,10 @@
         <v>39</v>
       </c>
       <c r="K30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2089,10 +2447,10 @@
         <v>39</v>
       </c>
       <c r="K31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -2124,10 +2482,10 @@
         <v>40</v>
       </c>
       <c r="K32" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -2159,10 +2517,10 @@
         <v>40</v>
       </c>
       <c r="K33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -2194,10 +2552,10 @@
         <v>40</v>
       </c>
       <c r="K34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2229,10 +2587,10 @@
         <v>41</v>
       </c>
       <c r="K35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2264,10 +2622,10 @@
         <v>41</v>
       </c>
       <c r="K36" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2299,10 +2657,10 @@
         <v>41</v>
       </c>
       <c r="K37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2334,10 +2692,10 @@
         <v>42</v>
       </c>
       <c r="K38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2369,10 +2727,10 @@
         <v>42</v>
       </c>
       <c r="K39" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2404,10 +2762,10 @@
         <v>42</v>
       </c>
       <c r="K40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2439,10 +2797,10 @@
         <v>43</v>
       </c>
       <c r="K41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2474,10 +2832,10 @@
         <v>43</v>
       </c>
       <c r="K42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2509,10 +2867,10 @@
         <v>43</v>
       </c>
       <c r="K43" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2544,10 +2902,10 @@
         <v>44</v>
       </c>
       <c r="K44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2579,10 +2937,10 @@
         <v>44</v>
       </c>
       <c r="K45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2614,10 +2972,10 @@
         <v>44</v>
       </c>
       <c r="K46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2649,10 +3007,10 @@
         <v>44</v>
       </c>
       <c r="K47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2684,10 +3042,10 @@
         <v>45</v>
       </c>
       <c r="K48" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2719,10 +3077,10 @@
         <v>45</v>
       </c>
       <c r="K49" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2754,10 +3112,10 @@
         <v>45</v>
       </c>
       <c r="K50" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2789,10 +3147,10 @@
         <v>46</v>
       </c>
       <c r="K51" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -2824,10 +3182,10 @@
         <v>46</v>
       </c>
       <c r="K52" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -2859,10 +3217,10 @@
         <v>46</v>
       </c>
       <c r="K53" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -2894,10 +3252,10 @@
         <v>47</v>
       </c>
       <c r="K54" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -2929,10 +3287,10 @@
         <v>47</v>
       </c>
       <c r="K55" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -2964,10 +3322,10 @@
         <v>47</v>
       </c>
       <c r="K56" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -2999,10 +3357,10 @@
         <v>48</v>
       </c>
       <c r="K57" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -3034,10 +3392,10 @@
         <v>48</v>
       </c>
       <c r="K58" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -3069,10 +3427,10 @@
         <v>48</v>
       </c>
       <c r="K59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -3104,10 +3462,10 @@
         <v>49</v>
       </c>
       <c r="K60" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -3139,10 +3497,10 @@
         <v>49</v>
       </c>
       <c r="K61" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -3174,10 +3532,10 @@
         <v>49</v>
       </c>
       <c r="K62" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -3209,10 +3567,10 @@
         <v>49</v>
       </c>
       <c r="K63" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -3244,10 +3602,10 @@
         <v>50</v>
       </c>
       <c r="K64" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -3279,10 +3637,10 @@
         <v>50</v>
       </c>
       <c r="K65" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3314,10 +3672,10 @@
         <v>50</v>
       </c>
       <c r="K66" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -3349,10 +3707,10 @@
         <v>51</v>
       </c>
       <c r="K67" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -3384,10 +3742,10 @@
         <v>51</v>
       </c>
       <c r="K68" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -3419,10 +3777,10 @@
         <v>51</v>
       </c>
       <c r="K69" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -3454,10 +3812,10 @@
         <v>52</v>
       </c>
       <c r="K70" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -3489,10 +3847,10 @@
         <v>52</v>
       </c>
       <c r="K71" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -3524,10 +3882,10 @@
         <v>52</v>
       </c>
       <c r="K72" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -3559,10 +3917,10 @@
         <v>52</v>
       </c>
       <c r="K73" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -3594,10 +3952,10 @@
         <v>52</v>
       </c>
       <c r="K74" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -3629,10 +3987,10 @@
         <v>52</v>
       </c>
       <c r="K75" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -3664,10 +4022,10 @@
         <v>52</v>
       </c>
       <c r="K76" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -3699,10 +4057,10 @@
         <v>52</v>
       </c>
       <c r="K77" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -3734,10 +4092,10 @@
         <v>52</v>
       </c>
       <c r="K78" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -3769,10 +4127,10 @@
         <v>52</v>
       </c>
       <c r="K79" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -3804,10 +4162,10 @@
         <v>53</v>
       </c>
       <c r="K80" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -3839,10 +4197,10 @@
         <v>53</v>
       </c>
       <c r="K81" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -3874,10 +4232,2940 @@
         <v>54</v>
       </c>
       <c r="K82" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="1">
+        <v>44495</v>
+      </c>
+      <c r="C83">
+        <v>2021</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>32.211068333333301</v>
+      </c>
+      <c r="F83">
+        <v>-111.00449</v>
+      </c>
+      <c r="G83">
+        <v>3063</v>
+      </c>
+      <c r="H83">
+        <v>21</v>
+      </c>
+      <c r="I83" t="s">
+        <v>23</v>
+      </c>
+      <c r="J83" t="s">
+        <v>54</v>
+      </c>
+      <c r="K83" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70659E3-6ADF-4861-A423-05040D976FDC}">
+  <dimension ref="A1:K83"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W18" sqref="W18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44467</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>32.248583333333301</v>
+      </c>
+      <c r="F2">
+        <v>-111.180433333333</v>
+      </c>
+      <c r="G2">
+        <v>2872</v>
+      </c>
+      <c r="H2">
+        <v>54</v>
+      </c>
+      <c r="I2">
+        <v>70</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44866</v>
+      </c>
+      <c r="C3">
+        <v>2022</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>32.248583333333301</v>
+      </c>
+      <c r="F3">
+        <v>-111.180433333333</v>
+      </c>
+      <c r="G3">
+        <v>2872</v>
+      </c>
+      <c r="H3">
+        <v>61</v>
+      </c>
+      <c r="I3">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44468</v>
+      </c>
+      <c r="C4">
+        <v>2021</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>32.248649999999998</v>
+      </c>
+      <c r="F4">
+        <v>-111.179683333333</v>
+      </c>
+      <c r="G4">
+        <v>2913</v>
+      </c>
+      <c r="H4">
+        <v>55</v>
+      </c>
+      <c r="I4">
+        <v>66</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44866</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>32.248649999999998</v>
+      </c>
+      <c r="F5">
+        <v>-111.179683333333</v>
+      </c>
+      <c r="G5">
+        <v>2913</v>
+      </c>
+      <c r="H5">
+        <v>62</v>
+      </c>
+      <c r="I5">
+        <v>66</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44451</v>
+      </c>
+      <c r="C6">
+        <v>2021</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>32.249016666666598</v>
+      </c>
+      <c r="F6">
+        <v>-111.17916666666601</v>
+      </c>
+      <c r="G6">
+        <v>2959</v>
+      </c>
+      <c r="H6">
+        <v>52</v>
+      </c>
+      <c r="I6">
+        <v>78</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44876</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>32.249016666666598</v>
+      </c>
+      <c r="F7">
+        <v>-111.17916666666601</v>
+      </c>
+      <c r="G7">
+        <v>2959</v>
+      </c>
+      <c r="H7">
+        <v>59</v>
+      </c>
+      <c r="I7">
+        <v>78</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44450</v>
+      </c>
+      <c r="C8">
+        <v>2021</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>32.249566666666603</v>
+      </c>
+      <c r="F8">
+        <v>-111.181166666666</v>
+      </c>
+      <c r="G8">
+        <v>2918</v>
+      </c>
+      <c r="H8">
+        <v>51</v>
+      </c>
+      <c r="I8">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44869</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>32.249566666666603</v>
+      </c>
+      <c r="F9">
+        <v>-111.181166666666</v>
+      </c>
+      <c r="G9">
+        <v>2918</v>
+      </c>
+      <c r="H9">
+        <v>58</v>
+      </c>
+      <c r="I9">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44450</v>
+      </c>
+      <c r="C10">
+        <v>2021</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>32.249049999999997</v>
+      </c>
+      <c r="F10">
+        <v>-111.181683333333</v>
+      </c>
+      <c r="G10">
+        <v>2836</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44869</v>
+      </c>
+      <c r="C11">
+        <v>2022</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>32.249049999999997</v>
+      </c>
+      <c r="F11">
+        <v>-111.181683333333</v>
+      </c>
+      <c r="G11">
+        <v>2836</v>
+      </c>
+      <c r="H11">
+        <v>57</v>
+      </c>
+      <c r="I11">
+        <v>76</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44451</v>
+      </c>
+      <c r="C12">
+        <v>2021</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>32.249033333333301</v>
+      </c>
+      <c r="F12">
+        <v>-111.17893333333301</v>
+      </c>
+      <c r="G12">
+        <v>2899</v>
+      </c>
+      <c r="H12">
+        <v>53</v>
+      </c>
+      <c r="I12">
+        <v>77</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44876</v>
+      </c>
+      <c r="C13">
+        <v>2022</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>32.249033333333301</v>
+      </c>
+      <c r="F13">
+        <v>-111.17893333333301</v>
+      </c>
+      <c r="G13">
+        <v>2899</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
+      <c r="I13">
+        <v>77</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44468</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>32.250133333333302</v>
+      </c>
+      <c r="F14">
+        <v>-111.1835</v>
+      </c>
+      <c r="G14">
+        <v>2783</v>
+      </c>
+      <c r="H14">
+        <v>56</v>
+      </c>
+      <c r="I14">
+        <v>68</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44876</v>
+      </c>
+      <c r="C15">
+        <v>2022</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>32.250133333333302</v>
+      </c>
+      <c r="F15">
+        <v>-111.1835</v>
+      </c>
+      <c r="G15">
+        <v>2783</v>
+      </c>
+      <c r="H15">
+        <v>63</v>
+      </c>
+      <c r="I15">
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44484</v>
+      </c>
+      <c r="C16">
+        <v>2021</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>32.283433333333299</v>
+      </c>
+      <c r="F16">
+        <v>-111.19218333333301</v>
+      </c>
+      <c r="G16">
+        <v>3052</v>
+      </c>
+      <c r="H16">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <v>84</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44845</v>
+      </c>
+      <c r="C17">
+        <v>2022</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>32.283433333333299</v>
+      </c>
+      <c r="F17">
+        <v>-111.19218333333301</v>
+      </c>
+      <c r="G17">
+        <v>3052</v>
+      </c>
+      <c r="H17">
+        <v>74</v>
+      </c>
+      <c r="I17">
+        <v>84</v>
+      </c>
+      <c r="J17" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45233</v>
+      </c>
+      <c r="C18">
+        <v>2023</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>32.283433333333299</v>
+      </c>
+      <c r="F18">
+        <v>-111.19218333333301</v>
+      </c>
+      <c r="G18">
+        <v>3052</v>
+      </c>
+      <c r="H18">
+        <v>81</v>
+      </c>
+      <c r="I18">
+        <v>84</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C19">
+        <v>2021</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>32.283783333333297</v>
+      </c>
+      <c r="F19">
+        <v>-111.19218333333301</v>
+      </c>
+      <c r="G19">
+        <v>3080</v>
+      </c>
+      <c r="H19">
+        <v>66</v>
+      </c>
+      <c r="I19">
+        <v>82</v>
+      </c>
+      <c r="J19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44851</v>
+      </c>
+      <c r="C20">
+        <v>2022</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>32.283783333333297</v>
+      </c>
+      <c r="F20">
+        <v>-111.19218333333301</v>
+      </c>
+      <c r="G20">
+        <v>3080</v>
+      </c>
+      <c r="H20">
+        <v>72</v>
+      </c>
+      <c r="I20">
+        <v>82</v>
+      </c>
+      <c r="J20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45226</v>
+      </c>
+      <c r="C21">
+        <v>2023</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>32.283783333333297</v>
+      </c>
+      <c r="F21">
+        <v>-111.19218333333301</v>
+      </c>
+      <c r="G21">
+        <v>3080</v>
+      </c>
+      <c r="H21">
+        <v>79</v>
+      </c>
+      <c r="I21">
+        <v>82</v>
+      </c>
+      <c r="J21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44477</v>
+      </c>
+      <c r="C22">
+        <v>2021</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>32.284266666666603</v>
+      </c>
+      <c r="F22">
+        <v>-111.190566666666</v>
+      </c>
+      <c r="G22">
+        <v>2802</v>
+      </c>
+      <c r="H22">
+        <v>69</v>
+      </c>
+      <c r="I22">
+        <v>85</v>
+      </c>
+      <c r="J22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44878</v>
+      </c>
+      <c r="C23">
+        <v>2022</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>32.284266666666603</v>
+      </c>
+      <c r="F23">
+        <v>-111.190566666666</v>
+      </c>
+      <c r="G23">
+        <v>2802</v>
+      </c>
+      <c r="H23">
+        <v>75</v>
+      </c>
+      <c r="I23">
+        <v>85</v>
+      </c>
+      <c r="J23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44852</v>
+      </c>
+      <c r="C24">
+        <v>2022</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>32.284266666666603</v>
+      </c>
+      <c r="F24">
+        <v>-111.190566666666</v>
+      </c>
+      <c r="G24">
+        <v>2802</v>
+      </c>
+      <c r="H24">
+        <v>76</v>
+      </c>
+      <c r="I24">
+        <v>85</v>
+      </c>
+      <c r="J24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45238</v>
+      </c>
+      <c r="C25">
+        <v>2023</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>32.284266666666603</v>
+      </c>
+      <c r="F25">
+        <v>-111.190566666666</v>
+      </c>
+      <c r="G25">
+        <v>2802</v>
+      </c>
+      <c r="H25">
+        <v>82</v>
+      </c>
+      <c r="I25">
+        <v>85</v>
+      </c>
+      <c r="J25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C26">
+        <v>2021</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>32.283933333333302</v>
+      </c>
+      <c r="F26">
+        <v>-111.1925</v>
+      </c>
+      <c r="G26">
+        <v>3042</v>
+      </c>
+      <c r="H26">
+        <v>67</v>
+      </c>
+      <c r="I26">
+        <v>83</v>
+      </c>
+      <c r="J26" t="s">
+        <v>38</v>
+      </c>
+      <c r="K26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44845</v>
+      </c>
+      <c r="C27">
+        <v>2022</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>32.283933333333302</v>
+      </c>
+      <c r="F27">
+        <v>-111.1925</v>
+      </c>
+      <c r="G27">
+        <v>3042</v>
+      </c>
+      <c r="H27">
+        <v>73</v>
+      </c>
+      <c r="I27">
+        <v>83</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45231</v>
+      </c>
+      <c r="C28">
+        <v>2023</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>32.283933333333302</v>
+      </c>
+      <c r="F28">
+        <v>-111.1925</v>
+      </c>
+      <c r="G28">
+        <v>3042</v>
+      </c>
+      <c r="H28">
+        <v>80</v>
+      </c>
+      <c r="I28">
+        <v>83</v>
+      </c>
+      <c r="J28" t="s">
+        <v>38</v>
+      </c>
+      <c r="K28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C29">
+        <v>2021</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>32.284216666666602</v>
+      </c>
+      <c r="F29">
+        <v>-111.191916666666</v>
+      </c>
+      <c r="G29">
+        <v>3067</v>
+      </c>
+      <c r="H29">
+        <v>65</v>
+      </c>
+      <c r="I29">
+        <v>80</v>
+      </c>
+      <c r="J29" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44851</v>
+      </c>
+      <c r="C30">
+        <v>2022</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>32.284216666666602</v>
+      </c>
+      <c r="F30">
+        <v>-111.191916666666</v>
+      </c>
+      <c r="G30">
+        <v>3067</v>
+      </c>
+      <c r="H30">
+        <v>71</v>
+      </c>
+      <c r="I30">
+        <v>80</v>
+      </c>
+      <c r="J30" t="s">
+        <v>39</v>
+      </c>
+      <c r="K30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45236</v>
+      </c>
+      <c r="C31">
+        <v>2023</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>32.284216666666602</v>
+      </c>
+      <c r="F31">
+        <v>-111.191916666666</v>
+      </c>
+      <c r="G31">
+        <v>3067</v>
+      </c>
+      <c r="H31">
+        <v>78</v>
+      </c>
+      <c r="I31">
+        <v>80</v>
+      </c>
+      <c r="J31" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44472</v>
+      </c>
+      <c r="C32">
+        <v>2021</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>32.284333333333301</v>
+      </c>
+      <c r="F32">
+        <v>-111.19308333333301</v>
+      </c>
+      <c r="G32">
+        <v>2991</v>
+      </c>
+      <c r="H32">
+        <v>64</v>
+      </c>
+      <c r="I32">
+        <v>79</v>
+      </c>
+      <c r="J32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44852</v>
+      </c>
+      <c r="C33">
+        <v>2022</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>32.284333333333301</v>
+      </c>
+      <c r="F33">
+        <v>-111.19308333333301</v>
+      </c>
+      <c r="G33">
+        <v>2991</v>
+      </c>
+      <c r="H33">
+        <v>70</v>
+      </c>
+      <c r="I33">
+        <v>79</v>
+      </c>
+      <c r="J33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45240</v>
+      </c>
+      <c r="C34">
+        <v>2023</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>32.284333333333301</v>
+      </c>
+      <c r="F34">
+        <v>-111.19308333333301</v>
+      </c>
+      <c r="G34">
+        <v>2991</v>
+      </c>
+      <c r="H34">
+        <v>77</v>
+      </c>
+      <c r="I34">
+        <v>79</v>
+      </c>
+      <c r="J34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44492</v>
+      </c>
+      <c r="C35">
+        <v>2021</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>32.191949999999999</v>
+      </c>
+      <c r="F35">
+        <v>-110.69806666666599</v>
+      </c>
+      <c r="G35">
+        <v>3324</v>
+      </c>
+      <c r="H35">
+        <v>41</v>
+      </c>
+      <c r="I35">
+        <v>71</v>
+      </c>
+      <c r="J35" t="s">
+        <v>41</v>
+      </c>
+      <c r="K35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44888</v>
+      </c>
+      <c r="C36">
+        <v>2022</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>32.191949999999999</v>
+      </c>
+      <c r="F36">
+        <v>-110.69806666666599</v>
+      </c>
+      <c r="G36">
+        <v>3324</v>
+      </c>
+      <c r="H36">
+        <v>44</v>
+      </c>
+      <c r="I36">
+        <v>71</v>
+      </c>
+      <c r="J36" t="s">
+        <v>41</v>
+      </c>
+      <c r="K36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45271</v>
+      </c>
+      <c r="C37">
+        <v>2023</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>32.191949999999999</v>
+      </c>
+      <c r="F37">
+        <v>-110.69806666666599</v>
+      </c>
+      <c r="G37">
+        <v>3324</v>
+      </c>
+      <c r="H37">
+        <v>47</v>
+      </c>
+      <c r="I37">
+        <v>71</v>
+      </c>
+      <c r="J37" t="s">
+        <v>41</v>
+      </c>
+      <c r="K37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44478</v>
+      </c>
+      <c r="C38">
+        <v>2021</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>32.191733333333303</v>
+      </c>
+      <c r="F38">
+        <v>-110.6965</v>
+      </c>
+      <c r="G38">
+        <v>3407</v>
+      </c>
+      <c r="H38">
+        <v>42</v>
+      </c>
+      <c r="I38">
+        <v>73</v>
+      </c>
+      <c r="J38" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44887</v>
+      </c>
+      <c r="C39">
+        <v>2022</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>32.191733333333303</v>
+      </c>
+      <c r="F39">
+        <v>-110.6965</v>
+      </c>
+      <c r="G39">
+        <v>3407</v>
+      </c>
+      <c r="H39">
+        <v>45</v>
+      </c>
+      <c r="I39">
+        <v>73</v>
+      </c>
+      <c r="J39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45273</v>
+      </c>
+      <c r="C40">
+        <v>2023</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>32.191733333333303</v>
+      </c>
+      <c r="F40">
+        <v>-110.6965</v>
+      </c>
+      <c r="G40">
+        <v>3407</v>
+      </c>
+      <c r="H40">
+        <v>48</v>
+      </c>
+      <c r="I40">
+        <v>73</v>
+      </c>
+      <c r="J40" t="s">
+        <v>42</v>
+      </c>
+      <c r="K40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44478</v>
+      </c>
+      <c r="C41">
+        <v>2021</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>32.1916333333333</v>
+      </c>
+      <c r="F41">
+        <v>-110.69629999999999</v>
+      </c>
+      <c r="G41">
+        <v>3443</v>
+      </c>
+      <c r="H41">
+        <v>43</v>
+      </c>
+      <c r="I41">
+        <v>74</v>
+      </c>
+      <c r="J41" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44887</v>
+      </c>
+      <c r="C42">
+        <v>2022</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>32.1916333333333</v>
+      </c>
+      <c r="F42">
+        <v>-110.69629999999999</v>
+      </c>
+      <c r="G42">
+        <v>3443</v>
+      </c>
+      <c r="H42">
+        <v>46</v>
+      </c>
+      <c r="I42">
+        <v>74</v>
+      </c>
+      <c r="J42" t="s">
+        <v>43</v>
+      </c>
+      <c r="K42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45275</v>
+      </c>
+      <c r="C43">
+        <v>2023</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>32.1916333333333</v>
+      </c>
+      <c r="F43">
+        <v>-110.69629999999999</v>
+      </c>
+      <c r="G43">
+        <v>3443</v>
+      </c>
+      <c r="H43">
+        <v>49</v>
+      </c>
+      <c r="I43">
+        <v>74</v>
+      </c>
+      <c r="J43" t="s">
+        <v>43</v>
+      </c>
+      <c r="K43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44105</v>
+      </c>
+      <c r="C44">
+        <v>2020</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>32.214983333333301</v>
+      </c>
+      <c r="F44">
+        <v>-111.00876666666601</v>
+      </c>
+      <c r="G44">
+        <v>2703</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44123</v>
+      </c>
+      <c r="C45">
+        <v>2020</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>32.214983333333301</v>
+      </c>
+      <c r="F45">
+        <v>-111.00876666666601</v>
+      </c>
+      <c r="G45">
+        <v>2703</v>
+      </c>
+      <c r="H45">
+        <v>9</v>
+      </c>
+      <c r="I45" t="s">
+        <v>13</v>
+      </c>
+      <c r="J45" t="s">
+        <v>44</v>
+      </c>
+      <c r="K45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44494</v>
+      </c>
+      <c r="C46">
+        <v>2021</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>32.214983333333301</v>
+      </c>
+      <c r="F46">
+        <v>-111.00876666666601</v>
+      </c>
+      <c r="G46">
+        <v>2703</v>
+      </c>
+      <c r="H46">
+        <v>20</v>
+      </c>
+      <c r="I46" t="s">
+        <v>13</v>
+      </c>
+      <c r="J46" t="s">
+        <v>44</v>
+      </c>
+      <c r="K46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44893</v>
+      </c>
+      <c r="C47">
+        <v>2022</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>32.214983333333301</v>
+      </c>
+      <c r="F47">
+        <v>-111.00876666666601</v>
+      </c>
+      <c r="G47">
+        <v>2703</v>
+      </c>
+      <c r="H47">
+        <v>37</v>
+      </c>
+      <c r="I47" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1">
+        <v>44123</v>
+      </c>
+      <c r="C48">
+        <v>2020</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>32.2124666666666</v>
+      </c>
+      <c r="F48">
+        <v>-111.00926666666599</v>
+      </c>
+      <c r="G48">
+        <v>2693</v>
+      </c>
+      <c r="H48">
+        <v>14</v>
+      </c>
+      <c r="I48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" t="s">
+        <v>45</v>
+      </c>
+      <c r="K48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1">
+        <v>44483</v>
+      </c>
+      <c r="C49">
+        <v>2021</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>32.2124666666666</v>
+      </c>
+      <c r="F49">
+        <v>-111.00926666666599</v>
+      </c>
+      <c r="G49">
+        <v>2693</v>
+      </c>
+      <c r="H49">
+        <v>25</v>
+      </c>
+      <c r="I49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" t="s">
+        <v>45</v>
+      </c>
+      <c r="K49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C50">
+        <v>2022</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>32.2124666666666</v>
+      </c>
+      <c r="F50">
+        <v>-111.00926666666599</v>
+      </c>
+      <c r="G50">
+        <v>2693</v>
+      </c>
+      <c r="H50">
+        <v>40</v>
+      </c>
+      <c r="I50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" t="s">
+        <v>45</v>
+      </c>
+      <c r="K50" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44105</v>
+      </c>
+      <c r="C51">
+        <v>2020</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>32.215583333333299</v>
+      </c>
+      <c r="F51">
+        <v>-111.008083333333</v>
+      </c>
+      <c r="G51">
+        <v>2805</v>
+      </c>
+      <c r="H51">
+        <v>7</v>
+      </c>
+      <c r="I51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J51" t="s">
+        <v>46</v>
+      </c>
+      <c r="K51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1">
+        <v>44464</v>
+      </c>
+      <c r="C52">
+        <v>2021</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>32.215583333333299</v>
+      </c>
+      <c r="F52">
+        <v>-111.008083333333</v>
+      </c>
+      <c r="G52">
+        <v>2805</v>
+      </c>
+      <c r="H52">
+        <v>19</v>
+      </c>
+      <c r="I52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" t="s">
+        <v>46</v>
+      </c>
+      <c r="K52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C53">
+        <v>2022</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53">
+        <v>32.215583333333299</v>
+      </c>
+      <c r="F53">
+        <v>-111.008083333333</v>
+      </c>
+      <c r="G53">
+        <v>2805</v>
+      </c>
+      <c r="H53">
+        <v>36</v>
+      </c>
+      <c r="I53" t="s">
+        <v>15</v>
+      </c>
+      <c r="J53" t="s">
+        <v>46</v>
+      </c>
+      <c r="K53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="1">
+        <v>44120</v>
+      </c>
+      <c r="C54">
+        <v>2020</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>32.217833333333303</v>
+      </c>
+      <c r="F54">
+        <v>-111.007483333333</v>
+      </c>
+      <c r="G54">
+        <v>2816</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" t="s">
+        <v>47</v>
+      </c>
+      <c r="K54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="1">
+        <v>44465</v>
+      </c>
+      <c r="C55">
+        <v>2021</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>32.217833333333303</v>
+      </c>
+      <c r="F55">
+        <v>-111.007483333333</v>
+      </c>
+      <c r="G55">
+        <v>2816</v>
+      </c>
+      <c r="H55">
+        <v>16</v>
+      </c>
+      <c r="I55" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" t="s">
+        <v>47</v>
+      </c>
+      <c r="K55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="1">
+        <v>44880</v>
+      </c>
+      <c r="C56">
+        <v>2022</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>32.217833333333303</v>
+      </c>
+      <c r="F56">
+        <v>-111.007483333333</v>
+      </c>
+      <c r="G56">
+        <v>2816</v>
+      </c>
+      <c r="H56">
+        <v>34</v>
+      </c>
+      <c r="I56" t="s">
+        <v>16</v>
+      </c>
+      <c r="J56" t="s">
+        <v>47</v>
+      </c>
+      <c r="K56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1">
+        <v>44102</v>
+      </c>
+      <c r="C57">
+        <v>2020</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>32.217616666666601</v>
+      </c>
+      <c r="F57">
+        <v>-111.007366666666</v>
+      </c>
+      <c r="G57">
+        <v>2830</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" t="s">
+        <v>48</v>
+      </c>
+      <c r="K57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1">
+        <v>44465</v>
+      </c>
+      <c r="C58">
+        <v>2021</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>32.217616666666601</v>
+      </c>
+      <c r="F58">
+        <v>-111.007366666666</v>
+      </c>
+      <c r="G58">
+        <v>2830</v>
+      </c>
+      <c r="H58">
+        <v>15</v>
+      </c>
+      <c r="I58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" t="s">
+        <v>48</v>
+      </c>
+      <c r="K58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="1">
+        <v>44880</v>
+      </c>
+      <c r="C59">
+        <v>2022</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59">
+        <v>32.217616666666601</v>
+      </c>
+      <c r="F59">
+        <v>-111.007366666666</v>
+      </c>
+      <c r="G59">
+        <v>2830</v>
+      </c>
+      <c r="H59">
+        <v>33</v>
+      </c>
+      <c r="I59" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" t="s">
+        <v>48</v>
+      </c>
+      <c r="K59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44104</v>
+      </c>
+      <c r="C60">
+        <v>2020</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>32.216266666666598</v>
+      </c>
+      <c r="F60">
+        <v>-111.006516666666</v>
+      </c>
+      <c r="G60">
+        <v>2885</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" t="s">
+        <v>49</v>
+      </c>
+      <c r="K60" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1">
+        <v>44102</v>
+      </c>
+      <c r="C61">
+        <v>2020</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>32.216266666666598</v>
+      </c>
+      <c r="F61">
+        <v>-111.006516666666</v>
+      </c>
+      <c r="G61">
+        <v>2885</v>
+      </c>
+      <c r="H61">
+        <v>6</v>
+      </c>
+      <c r="I61" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" t="s">
+        <v>49</v>
+      </c>
+      <c r="K61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44464</v>
+      </c>
+      <c r="C62">
+        <v>2021</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>32.216266666666598</v>
+      </c>
+      <c r="F62">
+        <v>-111.006516666666</v>
+      </c>
+      <c r="G62">
+        <v>2885</v>
+      </c>
+      <c r="H62">
+        <v>18</v>
+      </c>
+      <c r="I62" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" t="s">
+        <v>49</v>
+      </c>
+      <c r="K62" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44879</v>
+      </c>
+      <c r="C63">
+        <v>2022</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63">
+        <v>32.216266666666598</v>
+      </c>
+      <c r="F63">
+        <v>-111.006516666666</v>
+      </c>
+      <c r="G63">
+        <v>2885</v>
+      </c>
+      <c r="H63">
+        <v>35</v>
+      </c>
+      <c r="I63" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" t="s">
+        <v>49</v>
+      </c>
+      <c r="K63" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44117</v>
+      </c>
+      <c r="C64">
+        <v>2020</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>32.210349999999998</v>
+      </c>
+      <c r="F64">
+        <v>-111.00586666666599</v>
+      </c>
+      <c r="G64">
+        <v>2749</v>
+      </c>
+      <c r="H64">
+        <v>12</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J64" t="s">
+        <v>50</v>
+      </c>
+      <c r="K64" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="1">
+        <v>44479</v>
+      </c>
+      <c r="C65">
+        <v>2021</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>32.210349999999998</v>
+      </c>
+      <c r="F65">
+        <v>-111.00586666666599</v>
+      </c>
+      <c r="G65">
+        <v>2749</v>
+      </c>
+      <c r="H65">
+        <v>23</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65" t="s">
+        <v>50</v>
+      </c>
+      <c r="K65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C66">
+        <v>2022</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66">
+        <v>32.210349999999998</v>
+      </c>
+      <c r="F66">
+        <v>-111.00586666666599</v>
+      </c>
+      <c r="G66">
+        <v>2749</v>
+      </c>
+      <c r="H66">
+        <v>38</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66" t="s">
+        <v>50</v>
+      </c>
+      <c r="K66" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="1">
+        <v>44119</v>
+      </c>
+      <c r="C67">
+        <v>2020</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>32.209393333333303</v>
+      </c>
+      <c r="F67">
+        <v>-111.0061</v>
+      </c>
+      <c r="G67">
+        <v>2642</v>
+      </c>
+      <c r="H67">
+        <v>13</v>
+      </c>
+      <c r="I67" t="s">
+        <v>20</v>
+      </c>
+      <c r="J67" t="s">
+        <v>51</v>
+      </c>
+      <c r="K67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="1">
+        <v>44479</v>
+      </c>
+      <c r="C68">
+        <v>2021</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>32.209393333333303</v>
+      </c>
+      <c r="F68">
+        <v>-111.0061</v>
+      </c>
+      <c r="G68">
+        <v>2642</v>
+      </c>
+      <c r="H68">
+        <v>24</v>
+      </c>
+      <c r="I68" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68" t="s">
+        <v>51</v>
+      </c>
+      <c r="K68" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C69">
+        <v>2022</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69">
+        <v>32.209393333333303</v>
+      </c>
+      <c r="F69">
+        <v>-111.0061</v>
+      </c>
+      <c r="G69">
+        <v>2642</v>
+      </c>
+      <c r="H69">
+        <v>39</v>
+      </c>
+      <c r="I69" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" t="s">
+        <v>51</v>
+      </c>
+      <c r="K69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1">
+        <v>44103</v>
+      </c>
+      <c r="C70">
+        <v>2020</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F70">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G70">
+        <v>2775</v>
+      </c>
+      <c r="H70">
+        <v>3</v>
+      </c>
+      <c r="I70" t="s">
+        <v>21</v>
+      </c>
+      <c r="J70" t="s">
+        <v>52</v>
+      </c>
+      <c r="K70" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="1">
+        <v>44121</v>
+      </c>
+      <c r="C71">
+        <v>2020</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F71">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G71">
+        <v>2775</v>
+      </c>
+      <c r="H71">
+        <v>4</v>
+      </c>
+      <c r="I71" t="s">
+        <v>21</v>
+      </c>
+      <c r="J71" t="s">
+        <v>52</v>
+      </c>
+      <c r="K71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1">
+        <v>44463</v>
+      </c>
+      <c r="C72">
+        <v>2021</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F72">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G72">
+        <v>2775</v>
+      </c>
+      <c r="H72">
+        <v>17</v>
+      </c>
+      <c r="I72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J72" t="s">
+        <v>52</v>
+      </c>
+      <c r="K72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1">
+        <v>44496</v>
+      </c>
+      <c r="C73">
+        <v>2021</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F73">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G73">
+        <v>2775</v>
+      </c>
+      <c r="H73">
+        <v>26</v>
+      </c>
+      <c r="I73" t="s">
+        <v>21</v>
+      </c>
+      <c r="J73" t="s">
+        <v>52</v>
+      </c>
+      <c r="K73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="1">
+        <v>44501</v>
+      </c>
+      <c r="C74">
+        <v>2021</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F74">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G74">
+        <v>2775</v>
+      </c>
+      <c r="H74">
+        <v>27</v>
+      </c>
+      <c r="I74" t="s">
+        <v>21</v>
+      </c>
+      <c r="J74" t="s">
+        <v>52</v>
+      </c>
+      <c r="K74" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="1">
+        <v>44495</v>
+      </c>
+      <c r="C75">
+        <v>2021</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F75">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G75">
+        <v>2775</v>
+      </c>
+      <c r="H75">
+        <v>28</v>
+      </c>
+      <c r="I75" t="s">
+        <v>21</v>
+      </c>
+      <c r="J75" t="s">
+        <v>52</v>
+      </c>
+      <c r="K75" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="1">
+        <v>44497</v>
+      </c>
+      <c r="C76">
+        <v>2021</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F76">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G76">
+        <v>2775</v>
+      </c>
+      <c r="H76">
+        <v>29</v>
+      </c>
+      <c r="I76" t="s">
+        <v>21</v>
+      </c>
+      <c r="J76" t="s">
+        <v>52</v>
+      </c>
+      <c r="K76" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="1">
+        <v>44498</v>
+      </c>
+      <c r="C77">
+        <v>2021</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F77">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G77">
+        <v>2775</v>
+      </c>
+      <c r="H77">
+        <v>30</v>
+      </c>
+      <c r="I77" t="s">
+        <v>21</v>
+      </c>
+      <c r="J77" t="s">
+        <v>52</v>
+      </c>
+      <c r="K77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="1">
+        <v>44499</v>
+      </c>
+      <c r="C78">
+        <v>2021</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F78">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G78">
+        <v>2775</v>
+      </c>
+      <c r="H78">
+        <v>31</v>
+      </c>
+      <c r="I78" t="s">
+        <v>21</v>
+      </c>
+      <c r="J78" t="s">
+        <v>52</v>
+      </c>
+      <c r="K78" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="1">
+        <v>44500</v>
+      </c>
+      <c r="C79">
+        <v>2021</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>32.213833333333298</v>
+      </c>
+      <c r="F79">
+        <v>-111.002933333333</v>
+      </c>
+      <c r="G79">
+        <v>2775</v>
+      </c>
+      <c r="H79">
+        <v>32</v>
+      </c>
+      <c r="I79" t="s">
+        <v>21</v>
+      </c>
+      <c r="J79" t="s">
+        <v>52</v>
+      </c>
+      <c r="K79" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="1">
+        <v>44103</v>
+      </c>
+      <c r="C80">
+        <v>2020</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>32.214933333333299</v>
+      </c>
+      <c r="F80">
+        <v>-111.00213333333301</v>
+      </c>
+      <c r="G80">
+        <v>2711</v>
+      </c>
+      <c r="H80">
+        <v>11</v>
+      </c>
+      <c r="I80" t="s">
+        <v>22</v>
+      </c>
+      <c r="J80" t="s">
+        <v>53</v>
+      </c>
+      <c r="K80" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="1">
+        <v>44464</v>
+      </c>
+      <c r="C81">
+        <v>2021</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>32.214933333333299</v>
+      </c>
+      <c r="F81">
+        <v>-111.00213333333301</v>
+      </c>
+      <c r="G81">
+        <v>2711</v>
+      </c>
+      <c r="H81">
+        <v>22</v>
+      </c>
+      <c r="I81" t="s">
+        <v>22</v>
+      </c>
+      <c r="J81" t="s">
+        <v>53</v>
+      </c>
+      <c r="K81" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="1">
+        <v>44116</v>
+      </c>
+      <c r="C82">
+        <v>2020</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>32.211068333333301</v>
+      </c>
+      <c r="F82">
+        <v>-111.00449</v>
+      </c>
+      <c r="G82">
+        <v>3063</v>
+      </c>
+      <c r="H82">
+        <v>10</v>
+      </c>
+      <c r="I82" t="s">
+        <v>23</v>
+      </c>
+      <c r="J82" t="s">
+        <v>54</v>
+      </c>
+      <c r="K82" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -3919,7 +7207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CADEC49-775E-4106-A6D8-414B63D185D2}">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3927,14 +7215,14 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3957,7 +7245,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3980,7 +7268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4003,7 +7291,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -4026,7 +7314,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -4049,7 +7337,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -4072,7 +7360,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -4095,7 +7383,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -4118,7 +7406,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -4141,7 +7429,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4164,7 +7452,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4187,7 +7475,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -4210,7 +7498,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4233,7 +7521,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -4256,7 +7544,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -4279,7 +7567,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -4302,7 +7590,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -4325,7 +7613,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -4348,7 +7636,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -4371,7 +7659,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -4394,7 +7682,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -4417,7 +7705,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -4440,7 +7728,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -4463,7 +7751,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -4486,7 +7774,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -4509,7 +7797,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -4532,7 +7820,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -4555,7 +7843,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>

</xml_diff>